<commit_message>
V1.2 - graphs excel
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\dist agua\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\Condominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A564501-2D1B-4E14-8D7A-F0E5457B0AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79055F76-7CBD-4F90-A500-8BD3B226C251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>4) Criar uma senha de app</t>
   </si>
   <si>
-    <t>5) Copiar e colar na célula da planilha</t>
-  </si>
-  <si>
     <t>V1.0 7/24</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Obs: Qualquer alteração de edição das empresas na planilha emails deve também ser alterada na planilha "dados.xlsx".</t>
+  </si>
+  <si>
+    <t>5) Copiar e colar na célula da planilha. Caso possua espaços, é necessário retirar</t>
   </si>
 </sst>
 </file>
@@ -924,7 +924,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,42 +1017,42 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1082,17 +1082,17 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>